<commit_message>
more changes to align the municipalities between datasets
</commit_message>
<xml_diff>
--- a/hail/data/scenario_links.xlsx
+++ b/hail/data/scenario_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\berkhout\TIP\hail\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BAC88E-6CE6-4596-B0A2-9FABA21E1BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A30DC7-89AE-46B8-A5F4-402BCB9C1136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5445" windowWidth="38640" windowHeight="21840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47895" yWindow="-5325" windowWidth="19410" windowHeight="21705" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KM 2050" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,25 @@
     <sheet name="HA 2050" sheetId="7" r:id="rId7"/>
     <sheet name="HA 2040" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="397">
   <si>
     <t>GM0358</t>
   </si>
@@ -167,12 +180,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1327461</t>
   </si>
   <si>
-    <t>GM0416</t>
-  </si>
-  <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1327462</t>
-  </si>
-  <si>
     <t>GM0417</t>
   </si>
   <si>
@@ -239,12 +246,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1327473</t>
   </si>
   <si>
-    <t>GM0457</t>
-  </si>
-  <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1327474</t>
-  </si>
-  <si>
     <t>GM0473</t>
   </si>
   <si>
@@ -374,9 +375,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1327721</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1327722</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1327723</t>
   </si>
   <si>
@@ -410,9 +408,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1327733</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1327734</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1327783</t>
   </si>
   <si>
@@ -512,9 +507,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1327825</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1327826</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1327827</t>
   </si>
   <si>
@@ -548,9 +540,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1327837</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1327838</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1327839</t>
   </si>
   <si>
@@ -650,9 +639,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1327875</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1327876</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1327877</t>
   </si>
   <si>
@@ -686,9 +672,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1327887</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1327888</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1327889</t>
   </si>
   <si>
@@ -788,9 +771,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1328041</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1328042</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1328043</t>
   </si>
   <si>
@@ -824,9 +804,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1328053</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1328054</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1328055</t>
   </si>
   <si>
@@ -926,9 +903,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1327979</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1327980</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1327981</t>
   </si>
   <si>
@@ -962,9 +936,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1327991</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1327992</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1327993</t>
   </si>
   <si>
@@ -1064,9 +1035,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1328211</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1328212</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1328213</t>
   </si>
   <si>
@@ -1100,9 +1068,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1328223</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1328224</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1328225</t>
   </si>
   <si>
@@ -1202,9 +1167,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1328152</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1328153</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1328154</t>
   </si>
   <si>
@@ -1238,9 +1200,6 @@
     <t>https://pro.energytransitionmodel.com/scenarios/1328164</t>
   </si>
   <si>
-    <t>https://pro.energytransitionmodel.com/scenarios/1328165</t>
-  </si>
-  <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1328166</t>
   </si>
   <si>
@@ -1269,6 +1228,9 @@
   </si>
   <si>
     <t>https://pro.energytransitionmodel.com/scenarios/1328175</t>
+  </si>
+  <si>
+    <t>GM1980</t>
   </si>
 </sst>
 </file>
@@ -1608,10 +1570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1968,22 +1930,6 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>91</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1991,10 +1937,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2004,7 +1950,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2012,7 +1958,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2020,7 +1966,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2028,7 +1974,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2036,7 +1982,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2044,7 +1990,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2052,7 +1998,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2060,7 +2006,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2068,7 +2014,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2076,7 +2022,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2084,7 +2030,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2092,7 +2038,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2100,7 +2046,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2108,7 +2054,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2116,7 +2062,7 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -2124,15 +2070,15 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>396</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -2140,7 +2086,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -2148,7 +2094,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -2156,7 +2102,7 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2164,7 +2110,7 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -2172,7 +2118,7 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2180,7 +2126,7 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -2188,7 +2134,7 @@
         <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -2196,7 +2142,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -2204,7 +2150,7 @@
         <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -2212,7 +2158,7 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -2220,7 +2166,7 @@
         <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -2228,7 +2174,7 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -2236,7 +2182,7 @@
         <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -2244,7 +2190,7 @@
         <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -2252,7 +2198,7 @@
         <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -2260,7 +2206,7 @@
         <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -2268,7 +2214,7 @@
         <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -2276,7 +2222,7 @@
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -2284,7 +2230,7 @@
         <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -2292,7 +2238,7 @@
         <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -2300,7 +2246,7 @@
         <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2308,7 +2254,7 @@
         <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -2316,7 +2262,7 @@
         <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -2324,7 +2270,7 @@
         <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -2332,7 +2278,7 @@
         <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2340,7 +2286,7 @@
         <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -2348,23 +2294,7 @@
         <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2374,10 +2304,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2387,7 +2317,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2395,7 +2325,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2403,7 +2333,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2411,7 +2341,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2419,7 +2349,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2427,7 +2357,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2435,7 +2365,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2443,7 +2373,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2451,7 +2381,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2459,7 +2389,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2467,7 +2397,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2475,7 +2405,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2483,7 +2413,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2491,7 +2421,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2499,7 +2429,7 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -2507,15 +2437,15 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>396</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -2523,7 +2453,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -2531,7 +2461,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -2539,7 +2469,7 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2547,7 +2477,7 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -2555,7 +2485,7 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2563,7 +2493,7 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -2571,7 +2501,7 @@
         <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -2579,7 +2509,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -2587,7 +2517,7 @@
         <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -2595,7 +2525,7 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -2603,7 +2533,7 @@
         <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -2611,7 +2541,7 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -2619,7 +2549,7 @@
         <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -2627,7 +2557,7 @@
         <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -2635,7 +2565,7 @@
         <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -2643,7 +2573,7 @@
         <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -2651,7 +2581,7 @@
         <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -2659,7 +2589,7 @@
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -2667,7 +2597,7 @@
         <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -2675,7 +2605,7 @@
         <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -2683,7 +2613,7 @@
         <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2691,7 +2621,7 @@
         <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -2699,7 +2629,7 @@
         <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -2707,7 +2637,7 @@
         <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -2715,7 +2645,7 @@
         <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2723,7 +2653,7 @@
         <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -2731,23 +2661,7 @@
         <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2757,10 +2671,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2770,7 +2684,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2778,7 +2692,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2786,7 +2700,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2794,7 +2708,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2802,7 +2716,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2810,7 +2724,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2818,7 +2732,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2826,7 +2740,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2834,7 +2748,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2842,7 +2756,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2850,7 +2764,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2858,7 +2772,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2866,7 +2780,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2874,7 +2788,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2882,7 +2796,7 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -2890,15 +2804,15 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>396</v>
       </c>
       <c r="B17" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -2906,7 +2820,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -2914,7 +2828,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -2922,7 +2836,7 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2930,7 +2844,7 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -2938,7 +2852,7 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2946,7 +2860,7 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -2954,7 +2868,7 @@
         <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -2962,7 +2876,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -2970,7 +2884,7 @@
         <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -2978,7 +2892,7 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -2986,7 +2900,7 @@
         <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -2994,7 +2908,7 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -3002,7 +2916,7 @@
         <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -3010,7 +2924,7 @@
         <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -3018,7 +2932,7 @@
         <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -3026,7 +2940,7 @@
         <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -3034,7 +2948,7 @@
         <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -3042,7 +2956,7 @@
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -3050,7 +2964,7 @@
         <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -3058,7 +2972,7 @@
         <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -3066,7 +2980,7 @@
         <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -3074,7 +2988,7 @@
         <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -3082,7 +2996,7 @@
         <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -3090,7 +3004,7 @@
         <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -3098,7 +3012,7 @@
         <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -3106,7 +3020,7 @@
         <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -3114,23 +3028,7 @@
         <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -3140,10 +3038,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3153,7 +3051,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3161,7 +3059,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3169,7 +3067,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -3177,7 +3075,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -3185,7 +3083,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3193,7 +3091,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3201,7 +3099,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3209,7 +3107,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3217,7 +3115,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -3225,7 +3123,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3233,7 +3131,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -3241,7 +3139,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3249,7 +3147,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -3257,7 +3155,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -3265,7 +3163,7 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -3273,15 +3171,15 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>396</v>
       </c>
       <c r="B17" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -3289,7 +3187,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -3297,7 +3195,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -3305,7 +3203,7 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -3313,7 +3211,7 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -3321,7 +3219,7 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -3329,7 +3227,7 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -3337,7 +3235,7 @@
         <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -3345,7 +3243,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -3353,7 +3251,7 @@
         <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -3361,7 +3259,7 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -3369,7 +3267,7 @@
         <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -3377,7 +3275,7 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -3385,7 +3283,7 @@
         <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -3393,7 +3291,7 @@
         <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -3401,7 +3299,7 @@
         <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -3409,7 +3307,7 @@
         <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -3417,7 +3315,7 @@
         <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -3425,7 +3323,7 @@
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -3433,7 +3331,7 @@
         <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -3441,7 +3339,7 @@
         <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -3449,7 +3347,7 @@
         <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -3457,7 +3355,7 @@
         <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -3465,7 +3363,7 @@
         <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -3473,7 +3371,7 @@
         <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -3481,7 +3379,7 @@
         <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -3489,7 +3387,7 @@
         <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -3497,23 +3395,7 @@
         <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -3523,10 +3405,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3536,7 +3418,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3544,7 +3426,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3552,7 +3434,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -3560,7 +3442,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -3568,7 +3450,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3576,7 +3458,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3584,7 +3466,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3592,7 +3474,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3600,7 +3482,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -3608,7 +3490,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3616,7 +3498,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -3624,7 +3506,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3632,7 +3514,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -3640,7 +3522,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -3648,7 +3530,7 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -3656,15 +3538,15 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>396</v>
       </c>
       <c r="B17" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -3672,7 +3554,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -3680,7 +3562,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -3688,7 +3570,7 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -3696,7 +3578,7 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -3704,7 +3586,7 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -3712,7 +3594,7 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -3720,7 +3602,7 @@
         <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -3728,7 +3610,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -3736,7 +3618,7 @@
         <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -3744,7 +3626,7 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -3752,7 +3634,7 @@
         <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -3760,7 +3642,7 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -3768,7 +3650,7 @@
         <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -3776,7 +3658,7 @@
         <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -3784,7 +3666,7 @@
         <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -3792,7 +3674,7 @@
         <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -3800,7 +3682,7 @@
         <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -3808,7 +3690,7 @@
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -3816,7 +3698,7 @@
         <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -3824,7 +3706,7 @@
         <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -3832,7 +3714,7 @@
         <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -3840,7 +3722,7 @@
         <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -3848,7 +3730,7 @@
         <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -3856,7 +3738,7 @@
         <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -3864,7 +3746,7 @@
         <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -3872,7 +3754,7 @@
         <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -3880,23 +3762,7 @@
         <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -3906,10 +3772,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3919,7 +3785,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3927,7 +3793,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3935,7 +3801,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -3943,7 +3809,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -3951,7 +3817,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3959,7 +3825,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3967,7 +3833,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3975,7 +3841,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3983,7 +3849,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -3991,7 +3857,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3999,7 +3865,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -4007,7 +3873,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -4015,7 +3881,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -4023,7 +3889,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -4031,7 +3897,7 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -4039,15 +3905,15 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>396</v>
       </c>
       <c r="B17" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -4055,7 +3921,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -4063,7 +3929,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -4071,7 +3937,7 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -4079,7 +3945,7 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -4087,7 +3953,7 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -4095,7 +3961,7 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -4103,7 +3969,7 @@
         <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -4111,7 +3977,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -4119,7 +3985,7 @@
         <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -4127,7 +3993,7 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -4135,7 +4001,7 @@
         <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -4143,7 +4009,7 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -4151,7 +4017,7 @@
         <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -4159,7 +4025,7 @@
         <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -4167,7 +4033,7 @@
         <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4175,7 +4041,7 @@
         <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -4183,7 +4049,7 @@
         <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -4191,7 +4057,7 @@
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -4199,7 +4065,7 @@
         <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -4207,7 +4073,7 @@
         <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -4215,7 +4081,7 @@
         <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -4223,7 +4089,7 @@
         <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -4231,7 +4097,7 @@
         <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -4239,7 +4105,7 @@
         <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -4247,7 +4113,7 @@
         <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -4255,7 +4121,7 @@
         <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -4263,23 +4129,7 @@
         <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -4289,20 +4139,23 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -4310,7 +4163,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -4318,7 +4171,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4326,7 +4179,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4334,7 +4187,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4342,7 +4195,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4350,7 +4203,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -4358,7 +4211,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -4366,7 +4219,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -4374,7 +4227,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4382,7 +4235,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -4390,7 +4243,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -4398,7 +4251,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -4406,7 +4259,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -4414,7 +4267,7 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -4422,15 +4275,15 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>396</v>
       </c>
       <c r="B17" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -4438,7 +4291,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -4446,7 +4299,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -4454,7 +4307,7 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -4462,7 +4315,7 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -4470,7 +4323,7 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -4478,7 +4331,7 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -4486,7 +4339,7 @@
         <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -4494,7 +4347,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -4502,7 +4355,7 @@
         <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -4510,7 +4363,7 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -4518,7 +4371,7 @@
         <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -4526,7 +4379,7 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -4534,7 +4387,7 @@
         <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -4542,7 +4395,7 @@
         <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -4550,7 +4403,7 @@
         <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4558,7 +4411,7 @@
         <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -4566,7 +4419,7 @@
         <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -4574,7 +4427,7 @@
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -4582,7 +4435,7 @@
         <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -4590,7 +4443,7 @@
         <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -4598,7 +4451,7 @@
         <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -4606,7 +4459,7 @@
         <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -4614,7 +4467,7 @@
         <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -4622,7 +4475,7 @@
         <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -4630,7 +4483,7 @@
         <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -4638,7 +4491,7 @@
         <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -4646,23 +4499,7 @@
         <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>